<commit_message>
Neue Messung mit Standardabweichung
</commit_message>
<xml_diff>
--- a/bean-mapper-test/docs/jdk7/PerformanceTestWithCompleteFixtures.xlsx
+++ b/bean-mapper-test/docs/jdk7/PerformanceTestWithCompleteFixtures.xlsx
@@ -13,9 +13,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
-  <si>
-    <t>05.08.2014 um 17:16 Uhr</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
+  <si>
+    <t>02.08.2014 um 22:16 Uhr</t>
   </si>
   <si>
     <t>Name des Messpunkts</t>
@@ -33,7 +33,10 @@
     <t>Maximaler Messwert</t>
   </si>
   <si>
-    <t>Mittelwert</t>
+    <t>Arth. Mittelwert</t>
+  </si>
+  <si>
+    <t>Standardabweichung</t>
   </si>
   <si>
     <t>Letzter Messwert</t>
@@ -49,6 +52,9 @@
   </si>
   <si>
     <t>MapStruct</t>
+  </si>
+  <si>
+    <t>Messreihen</t>
   </si>
 </sst>
 </file>
@@ -107,7 +113,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
-      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -140,10 +146,13 @@
       <c r="G2" t="s" s="1">
         <v>7</v>
       </c>
+      <c r="H2" t="s" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="n">
         <v>10.0</v>
@@ -160,65 +169,74 @@
       <c r="F3" t="n" s="2">
         <v>1.7</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" t="n" s="2">
+        <v>0.483046</v>
+      </c>
+      <c r="H3" t="n">
         <v>2.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n">
         <v>10.0</v>
       </c>
       <c r="C4" t="n">
-        <v>856.0</v>
+        <v>950.0</v>
       </c>
       <c r="D4" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="E4" t="n">
         <v>405.0</v>
       </c>
       <c r="F4" t="n" s="2">
-        <v>85.6</v>
-      </c>
-      <c r="G4" t="n">
-        <v>27.0</v>
+        <v>95.0</v>
+      </c>
+      <c r="G4" t="n" s="2">
+        <v>119.139</v>
+      </c>
+      <c r="H4" t="n">
+        <v>28.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="n">
         <v>10.0</v>
       </c>
       <c r="C5" t="n">
-        <v>281.0</v>
+        <v>289.0</v>
       </c>
       <c r="D5" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E5" t="n">
         <v>242.0</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>28.1</v>
-      </c>
-      <c r="G5" t="n">
-        <v>3.0</v>
+        <v>28.9</v>
+      </c>
+      <c r="G5" t="n" s="2">
+        <v>74.8813</v>
+      </c>
+      <c r="H5" t="n">
+        <v>5.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="n">
         <v>10.0</v>
       </c>
       <c r="C6" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
       <c r="D6" t="n">
         <v>1.0</v>
@@ -227,10 +245,13 @@
         <v>4.0</v>
       </c>
       <c r="F6" t="n" s="2">
-        <v>2.1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1.0</v>
+        <v>2.2</v>
+      </c>
+      <c r="G6" t="n" s="2">
+        <v>0.788811</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>
@@ -276,62 +297,71 @@
       <c r="G2" t="s" s="1">
         <v>7</v>
       </c>
+      <c r="H2" t="s" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>50874.0</v>
+        <v>51774.0</v>
       </c>
       <c r="C3" t="n">
-        <v>997.0</v>
+        <v>980.0</v>
       </c>
       <c r="D3" t="n">
         <v>0.0</v>
       </c>
       <c r="E3" t="n">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
       <c r="F3" t="n" s="2">
-        <v>0.019597</v>
-      </c>
-      <c r="G3" t="n">
+        <v>0.0189284</v>
+      </c>
+      <c r="G3" t="n" s="2">
+        <v>0.147176</v>
+      </c>
+      <c r="H3" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>50874.0</v>
+        <v>51774.0</v>
       </c>
       <c r="C4" t="n">
-        <v>534590.0</v>
+        <v>532851.0</v>
       </c>
       <c r="D4" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="E4" t="n">
-        <v>83.0</v>
+        <v>34.0</v>
       </c>
       <c r="F4" t="n" s="2">
-        <v>10.508</v>
-      </c>
-      <c r="G4" t="n">
+        <v>10.2919</v>
+      </c>
+      <c r="G4" t="n" s="2">
+        <v>1.1458</v>
+      </c>
+      <c r="H4" t="n">
         <v>10.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>50874.0</v>
+        <v>51774.0</v>
       </c>
       <c r="C5" t="n">
-        <v>26733.0</v>
+        <v>27363.0</v>
       </c>
       <c r="D5" t="n">
         <v>0.0</v>
@@ -340,36 +370,45 @@
         <v>15.0</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>0.52547</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.0</v>
+        <v>0.528509</v>
+      </c>
+      <c r="G5" t="n" s="2">
+        <v>0.547114</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="n">
-        <v>50874.0</v>
+        <v>51774.0</v>
       </c>
       <c r="C6" t="n">
-        <v>13949.0</v>
+        <v>14732.0</v>
       </c>
       <c r="D6" t="n">
         <v>0.0</v>
       </c>
       <c r="E6" t="n">
-        <v>12.0</v>
+        <v>4.0</v>
       </c>
       <c r="F6" t="n" s="2">
-        <v>0.27419</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1.0</v>
+        <v>0.284544</v>
+      </c>
+      <c r="G6" t="n" s="2">
+        <v>0.458884</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
+      <c r="A9" t="s" s="1">
+        <v>13</v>
+      </c>
       <c r="B9" t="n" s="1">
         <v>10.0</v>
       </c>
@@ -397,118 +436,118 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="n" s="2">
         <v>1.4</v>
       </c>
       <c r="C10" t="n" s="2">
-        <v>0.63</v>
+        <v>0.59</v>
       </c>
       <c r="D10" t="n" s="2">
-        <v>0.083</v>
+        <v>0.068</v>
       </c>
       <c r="E10" t="n" s="2">
-        <v>0.0236</v>
+        <v>0.0234</v>
       </c>
       <c r="F10" t="n" s="2">
-        <v>0.02035</v>
+        <v>0.0213</v>
       </c>
       <c r="G10" t="n" s="2">
-        <v>0.0197</v>
+        <v>0.0200667</v>
       </c>
       <c r="H10" t="n" s="2">
-        <v>0.019375</v>
+        <v>0.01955</v>
       </c>
       <c r="I10" t="n" s="2">
-        <v>0.0196</v>
+        <v>0.01906</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="n" s="2">
-        <v>22.6</v>
+        <v>23.4</v>
       </c>
       <c r="C11" t="n" s="2">
-        <v>19.62</v>
+        <v>18.94</v>
       </c>
       <c r="D11" t="n" s="2">
-        <v>11.315</v>
+        <v>11.18</v>
       </c>
       <c r="E11" t="n" s="2">
-        <v>10.401</v>
+        <v>10.3857</v>
       </c>
       <c r="F11" t="n" s="2">
-        <v>10.388</v>
+        <v>10.3307</v>
       </c>
       <c r="G11" t="n" s="2">
-        <v>10.391</v>
+        <v>10.3024</v>
       </c>
       <c r="H11" t="n" s="2">
-        <v>10.437</v>
+        <v>10.2938</v>
       </c>
       <c r="I11" t="n" s="2">
-        <v>10.508</v>
+        <v>10.2909</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="n" s="2">
-        <v>3.8</v>
+        <v>3.9</v>
       </c>
       <c r="C12" t="n" s="2">
-        <v>2.56</v>
+        <v>2.78</v>
       </c>
       <c r="D12" t="n" s="2">
-        <v>0.72</v>
+        <v>0.754</v>
       </c>
       <c r="E12" t="n" s="2">
-        <v>0.5307</v>
+        <v>0.5519</v>
       </c>
       <c r="F12" t="n" s="2">
-        <v>0.523</v>
+        <v>0.54005</v>
       </c>
       <c r="G12" t="n" s="2">
-        <v>0.521</v>
+        <v>0.531933</v>
       </c>
       <c r="H12" t="n" s="2">
-        <v>0.5227</v>
+        <v>0.529425</v>
       </c>
       <c r="I12" t="n" s="2">
-        <v>0.52556</v>
+        <v>0.52892</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="n" s="2">
         <v>1.7</v>
       </c>
       <c r="C13" t="n" s="2">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="D13" t="n" s="2">
-        <v>0.364</v>
+        <v>0.391</v>
       </c>
       <c r="E13" t="n" s="2">
-        <v>0.2818</v>
+        <v>0.3009</v>
       </c>
       <c r="F13" t="n" s="2">
-        <v>0.2728</v>
+        <v>0.28565</v>
       </c>
       <c r="G13" t="n" s="2">
-        <v>0.2706</v>
+        <v>0.286933</v>
       </c>
       <c r="H13" t="n" s="2">
-        <v>0.27198</v>
+        <v>0.286575</v>
       </c>
       <c r="I13" t="n" s="2">
-        <v>0.27424</v>
+        <v>0.2844</v>
       </c>
     </row>
   </sheetData>

</xml_diff>